<commit_message>
Infaq abu zain 2jt
</commit_message>
<xml_diff>
--- a/Penggalangan Dana Pembangunan Gedung Banin - Banat MDS.xlsx
+++ b/Penggalangan Dana Pembangunan Gedung Banin - Banat MDS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="23895" windowHeight="10350"/>
   </bookViews>
   <sheets>
     <sheet name="Banin - Banat" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74">
   <si>
     <t>Penggalangan Dana Pembangunan Gedung Banin - Banat MDS</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Hamba Allah via Abu Thalhah</t>
+  </si>
+  <si>
+    <t>Abu Zain Cilacap</t>
   </si>
   <si>
     <t>Penggalangan Dana Pembangunan Kanopi &amp; Penyempurnaan Masjid Ibnu Taimiyah</t>
@@ -244,11 +247,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -268,21 +271,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -296,15 +285,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -313,14 +293,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -334,17 +307,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -367,7 +340,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -378,6 +358,14 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -406,6 +394,21 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -444,7 +447,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -456,13 +483,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,31 +609,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,121 +621,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -818,41 +821,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -873,6 +841,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -900,14 +883,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -919,134 +922,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1062,22 +1065,23 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -1111,7 +1115,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1897,10 +1901,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1941,12 +1945,12 @@
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="14"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="22" t="s">
+      <c r="J2" s="22"/>
+      <c r="K2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="23"/>
-      <c r="N2" s="24" t="s">
+      <c r="L2" s="24"/>
+      <c r="N2" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1975,16 +1979,16 @@
       <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="27">
+      <c r="N3" s="28">
         <v>397597</v>
       </c>
     </row>
@@ -2012,14 +2016,14 @@
         <f>F4-G4</f>
         <v>100000</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="29">
+      <c r="K4" s="30">
         <v>16669000</v>
       </c>
-      <c r="L4" s="30"/>
-      <c r="N4" s="31">
+      <c r="L4" s="31"/>
+      <c r="N4" s="32">
         <f>N3-250000</f>
         <v>147597</v>
       </c>
@@ -2048,13 +2052,13 @@
         <f>H4+F5-G5</f>
         <v>600000</v>
       </c>
-      <c r="J5" s="32" t="s">
+      <c r="J5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="33">
+      <c r="K5" s="34">
         <v>20500000</v>
       </c>
-      <c r="L5" s="34"/>
+      <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="5">
@@ -2080,11 +2084,11 @@
         <f>H5+F6-G6</f>
         <v>10600000</v>
       </c>
-      <c r="J6" s="32" t="s">
+      <c r="J6" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="35"/>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="5">
@@ -2110,14 +2114,14 @@
         <f t="shared" ref="H7:H39" si="0">H6+F7-G7</f>
         <v>11600000</v>
       </c>
-      <c r="J7" s="35" t="s">
+      <c r="J7" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="36">
+      <c r="K7" s="37">
         <v>37169000</v>
       </c>
-      <c r="L7" s="37"/>
-      <c r="N7" s="31"/>
+      <c r="L7" s="38"/>
+      <c r="N7" s="32"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5">
@@ -2168,7 +2172,7 @@
         <f t="shared" si="0"/>
         <v>11850000</v>
       </c>
-      <c r="N9" s="38">
+      <c r="N9" s="39">
         <v>-147597</v>
       </c>
     </row>
@@ -2196,19 +2200,19 @@
         <f t="shared" si="0"/>
         <v>12450000</v>
       </c>
-      <c r="J10" s="39" t="s">
+      <c r="J10" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="K10" s="40" t="s">
+      <c r="K10" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="L10" s="40" t="s">
+      <c r="L10" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="40" t="s">
+      <c r="M10" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="41" t="s">
+      <c r="N10" s="42" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2281,7 +2285,7 @@
         <f t="shared" si="0"/>
         <v>13516000</v>
       </c>
-      <c r="N12" s="38"/>
+      <c r="N12" s="39"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="5">
@@ -2332,7 +2336,7 @@
         <f t="shared" si="0"/>
         <v>20516000</v>
       </c>
-      <c r="N14" s="31"/>
+      <c r="N14" s="32"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="5">
@@ -2408,7 +2412,7 @@
         <f t="shared" si="0"/>
         <v>21066000</v>
       </c>
-      <c r="L17" s="42"/>
+      <c r="L17" s="43"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="5">
@@ -2926,7 +2930,7 @@
       <c r="E38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="19">
         <v>100000</v>
       </c>
       <c r="G38" s="5"/>
@@ -2936,28 +2940,222 @@
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="19">
+      <c r="A39" s="5">
         <v>36</v>
       </c>
-      <c r="B39" s="20">
+      <c r="B39" s="6">
         <v>42860</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F39" s="19">
         <v>50000</v>
       </c>
-      <c r="G39" s="19"/>
+      <c r="G39" s="5"/>
       <c r="H39" s="7">
         <f t="shared" si="0"/>
         <v>37319000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="5">
+        <v>37</v>
+      </c>
+      <c r="B40" s="6">
+        <v>42860</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="21">
+        <v>2000000</v>
+      </c>
+      <c r="G40" s="20"/>
+      <c r="H40" s="7">
+        <f t="shared" ref="H40:H53" si="1">H39+F40-G40</f>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="20"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="20"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="20"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="20"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="20"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="20"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50" s="20"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51" s="20"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="A52" s="20"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="7">
+        <f t="shared" si="1"/>
+        <v>39319000</v>
       </c>
     </row>
   </sheetData>
@@ -2992,7 +3190,7 @@
   <sheetData>
     <row r="1" ht="32.25" customHeight="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3101,7 +3299,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>14</v>
@@ -3151,7 +3349,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>14</v>
@@ -3201,7 +3399,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>15</v>
@@ -3251,7 +3449,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>15</v>
@@ -3273,13 +3471,13 @@
         <v>42856</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F13" s="11"/>
       <c r="G13" s="11">
@@ -3301,7 +3499,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>15</v>
@@ -3326,7 +3524,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>15</v>
@@ -3373,10 +3571,10 @@
         <v>42858</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
update dana pembangunan,penerimaan spp, biaya mahad
</commit_message>
<xml_diff>
--- a/Penggalangan Dana Pembangunan Gedung Banin - Banat MDS.xlsx
+++ b/Penggalangan Dana Pembangunan Gedung Banin - Banat MDS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370" firstSheet="1" activeTab="5"/>
+    <workbookView windowWidth="19890" windowHeight="8370" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Banin - Banat" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259">
   <si>
     <t>Penggalangan Dana Pembangunan Gedung Banin - Banat MDS</t>
   </si>
@@ -653,6 +653,9 @@
   </si>
   <si>
     <t>KW : 2782</t>
+  </si>
+  <si>
+    <t>Andjon Djatim , Musyahadah</t>
   </si>
   <si>
     <t>Masjid</t>
@@ -806,14 +809,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="m/d/yy\ h:mm\ AM/PM;@"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="m/d/yyyy;@"/>
-    <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="180" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -859,6 +862,7 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -867,14 +871,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -888,26 +908,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -919,15 +939,16 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -941,40 +962,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -995,11 +984,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1066,7 +1069,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1078,13 +1153,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1096,85 +1213,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1192,37 +1231,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1235,12 +1244,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1418,17 +1421,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1442,31 +1441,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1515,14 +1500,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1534,130 +1537,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="35" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1753,7 +1756,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="180" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="177" fontId="0" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="58" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1780,7 +1783,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="180" fontId="1" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="177" fontId="1" fillId="6" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1798,7 +1801,7 @@
     <xf numFmtId="177" fontId="1" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1811,7 +1814,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
@@ -1835,7 +1838,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -11013,8 +11016,8 @@
   <sheetPr/>
   <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView topLeftCell="B47" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.12380952380952" defaultRowHeight="15"/>
@@ -12386,7 +12389,7 @@
       </c>
       <c r="L40" s="75">
         <f>I67-J67</f>
-        <v>22730000</v>
+        <v>23730000</v>
       </c>
     </row>
     <row r="41" s="75" customFormat="1" spans="1:11">
@@ -13083,18 +13086,28 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B65" s="71"/>
-      <c r="C65" s="70"/>
-      <c r="D65" s="70"/>
-      <c r="E65" s="70"/>
+      <c r="B65" s="71">
+        <v>43155</v>
+      </c>
+      <c r="C65" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="D65" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="E65" s="70" t="s">
+        <v>14</v>
+      </c>
       <c r="F65" s="70"/>
       <c r="G65" s="72"/>
       <c r="H65" s="72"/>
-      <c r="I65" s="72"/>
+      <c r="I65" s="72">
+        <v>1000000</v>
+      </c>
       <c r="J65" s="72"/>
       <c r="K65" s="72">
         <f t="shared" si="8"/>
-        <v>22730000</v>
+        <v>23730000</v>
       </c>
     </row>
     <row r="66" s="75" customFormat="1" spans="1:11">
@@ -13113,7 +13126,7 @@
       <c r="J66" s="72"/>
       <c r="K66" s="72">
         <f t="shared" si="8"/>
-        <v>22730000</v>
+        <v>23730000</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -13123,7 +13136,7 @@
       </c>
       <c r="I67" s="59">
         <f>SUM(I4:I66)</f>
-        <v>77174000</v>
+        <v>78174000</v>
       </c>
       <c r="J67" s="59">
         <f>SUM(J4:J66)</f>
@@ -13163,10 +13176,10 @@
         <v>67</v>
       </c>
       <c r="G70" s="80" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H70" s="80" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -13314,7 +13327,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="67" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -13527,7 +13540,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="73" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C9" s="34" t="s">
         <v>13</v>
@@ -13620,7 +13633,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E12" s="70" t="s">
         <v>19</v>
@@ -13646,7 +13659,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E13" s="70" t="s">
         <v>14</v>
@@ -13672,10 +13685,10 @@
         <v>43090</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E14" s="70" t="s">
         <v>14</v>
@@ -13730,10 +13743,10 @@
         <v>43097</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>19</v>
@@ -13759,7 +13772,7 @@
         <v>43100</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D17" s="34"/>
       <c r="E17" s="34" t="s">
@@ -13844,10 +13857,10 @@
         <v>43102</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E20" s="34" t="s">
         <v>19</v>
@@ -13873,10 +13886,10 @@
         <v>43102</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="E21" s="34" t="s">
         <v>19</v>
@@ -13902,10 +13915,10 @@
         <v>43102</v>
       </c>
       <c r="C22" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E22" s="34" t="s">
         <v>19</v>
@@ -13960,10 +13973,10 @@
         <v>43113</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E24" s="34" t="s">
         <v>19</v>
@@ -13989,10 +14002,10 @@
         <v>43113</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E25" s="34" t="s">
         <v>19</v>
@@ -14018,7 +14031,7 @@
         <v>43138</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D26" s="34"/>
       <c r="E26" s="34" t="s">
@@ -14046,7 +14059,7 @@
         <v>43138</v>
       </c>
       <c r="C27" s="34" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D27" s="34"/>
       <c r="E27" s="34" t="s">
@@ -14105,10 +14118,10 @@
         <v>13</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="34"/>
@@ -14134,7 +14147,7 @@
         <v>13</v>
       </c>
       <c r="D30" s="34" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E30" s="34" t="s">
         <v>19</v>
@@ -14163,7 +14176,7 @@
         <v>13</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E31" s="34" t="s">
         <v>19</v>
@@ -14265,7 +14278,7 @@
   <sheetPr/>
   <dimension ref="B2:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -14287,7 +14300,7 @@
   <sheetData>
     <row r="2" spans="2:10">
       <c r="B2" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -14302,7 +14315,7 @@
     <row r="3" spans="2:10">
       <c r="B3" s="8" t="str">
         <f ca="1">CONCATENATE("Per : "," ",TEXT(NOW(),"DD/MM/YYYY hh:mm:ss"))</f>
-        <v>Per :  22/02/2018 22:35:00</v>
+        <v>Per :  26/02/2018 06:45:29</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -14310,7 +14323,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="11"/>
       <c r="H3" s="12" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I3" s="56"/>
       <c r="J3" s="56" t="s">
@@ -14325,7 +14338,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="16"/>
       <c r="H4" s="17" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="I4" s="57"/>
       <c r="J4" s="58">
@@ -14339,28 +14352,28 @@
     </row>
     <row r="5" ht="32.25" customHeight="1" spans="2:11">
       <c r="B5" s="18" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="21" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I5" s="60"/>
       <c r="J5" s="61">
         <f>F33</f>
-        <v>12730000</v>
+        <v>13730000</v>
       </c>
       <c r="K5" s="59">
         <f>1547797+38000000</f>
@@ -14369,25 +14382,25 @@
     </row>
     <row r="6" spans="2:11">
       <c r="B6" s="22" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C6" s="23">
         <v>99000000</v>
       </c>
       <c r="D6" s="23">
         <f>MTS!K66</f>
-        <v>22730000</v>
+        <v>23730000</v>
       </c>
       <c r="E6" s="24">
         <f>D6/C6</f>
-        <v>0.22959595959596</v>
+        <v>0.23969696969697</v>
       </c>
       <c r="F6" s="23">
         <f>C6-D6</f>
-        <v>76270000</v>
+        <v>75270000</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I6" s="34"/>
       <c r="J6" s="61">
@@ -14401,7 +14414,7 @@
     </row>
     <row r="7" ht="15.75" spans="2:11">
       <c r="B7" s="26" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C7" s="27">
         <v>150000000</v>
@@ -14419,12 +14432,12 @@
         <v>114049400</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="I7" s="62"/>
       <c r="J7" s="63">
         <f>SUM(J4:J6)</f>
-        <v>53512900</v>
+        <v>54512900</v>
       </c>
       <c r="K7" s="59">
         <f>SUM(K4:K6)</f>
@@ -14433,7 +14446,7 @@
     </row>
     <row r="8" ht="15.75" spans="2:11">
       <c r="B8" s="29" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C8" s="30">
         <f>SUM(C6:C7)</f>
@@ -14441,22 +14454,22 @@
       </c>
       <c r="D8" s="30">
         <f>SUM(D6:D7)</f>
-        <v>58680600</v>
+        <v>59680600</v>
       </c>
       <c r="E8" s="31">
         <f>D8/C8</f>
-        <v>0.235665060240964</v>
+        <v>0.239681124497992</v>
       </c>
       <c r="F8" s="30">
         <f>C8-D8</f>
-        <v>190319400</v>
+        <v>189319400</v>
       </c>
       <c r="H8" s="32"/>
       <c r="K8" s="64"/>
     </row>
     <row r="9" spans="2:11">
       <c r="B9" s="33" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C9" s="33"/>
       <c r="D9" s="33"/>
@@ -14465,7 +14478,7 @@
       <c r="H9" s="32"/>
       <c r="K9" s="59">
         <f>K7-D8</f>
-        <v>-5281803</v>
+        <v>-6281803</v>
       </c>
     </row>
     <row r="10" spans="2:10">
@@ -14475,7 +14488,7 @@
       <c r="E10" s="33"/>
       <c r="F10" s="33"/>
       <c r="H10" s="21" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
@@ -14487,7 +14500,7 @@
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
       <c r="H11" s="34" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="I11" s="34"/>
       <c r="J11" s="61">
@@ -14496,7 +14509,7 @@
     </row>
     <row r="12" hidden="1" spans="2:10">
       <c r="B12" s="161" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
@@ -14508,14 +14521,14 @@
     </row>
     <row r="13" spans="2:15">
       <c r="B13" s="35" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
       <c r="E13" s="36"/>
       <c r="F13" s="36"/>
       <c r="H13" s="25" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I13" s="34"/>
       <c r="J13" s="61">
@@ -14554,7 +14567,7 @@
       <c r="E16" s="36"/>
       <c r="F16" s="36"/>
       <c r="H16" s="21" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="I16" s="62"/>
       <c r="J16" s="63">
@@ -14577,11 +14590,11 @@
       <c r="E18" s="36"/>
       <c r="F18" s="36"/>
       <c r="H18" s="32" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J18" s="66">
         <f>J16-J7</f>
-        <v>1300000</v>
+        <v>300000</v>
       </c>
     </row>
     <row r="19" spans="2:10">
@@ -14606,7 +14619,7 @@
     </row>
     <row r="22" spans="2:6">
       <c r="B22" s="5" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -14616,7 +14629,7 @@
     <row r="23" spans="2:6">
       <c r="B23" s="8" t="str">
         <f ca="1">CONCATENATE("Per : "," ",TEXT(NOW(),"DD/MM/YYYY hh:mm:ss"))</f>
-        <v>Per :  22/02/2018 22:35:00</v>
+        <v>Per :  26/02/2018 06:45:29</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -14632,13 +14645,13 @@
     </row>
     <row r="25" spans="2:6">
       <c r="B25" s="37" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C25" s="37" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E25" s="37" t="s">
         <v>2</v>
@@ -14649,14 +14662,14 @@
     </row>
     <row r="26" ht="30" spans="2:6">
       <c r="B26" s="38" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C26" s="39">
         <f>D6</f>
-        <v>22730000</v>
+        <v>23730000</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E26" s="41">
         <v>43113</v>
@@ -14669,7 +14682,7 @@
       <c r="B27" s="42"/>
       <c r="C27" s="43"/>
       <c r="D27" s="40" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E27" s="44">
         <v>43148</v>
@@ -14710,7 +14723,7 @@
       <c r="B32" s="46"/>
       <c r="C32" s="47"/>
       <c r="D32" s="48" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E32" s="49"/>
       <c r="F32" s="50">
@@ -14722,27 +14735,27 @@
       <c r="B33" s="51"/>
       <c r="C33" s="52"/>
       <c r="D33" s="53" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E33" s="54"/>
       <c r="F33" s="55">
         <f>C34-F32</f>
-        <v>12730000</v>
+        <v>13730000</v>
       </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="49" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C34" s="50">
         <f>SUM(C26:C33)</f>
-        <v>22730000</v>
+        <v>23730000</v>
       </c>
       <c r="D34" s="48"/>
       <c r="E34" s="49"/>
       <c r="F34" s="50">
         <f>F32+F33</f>
-        <v>22730000</v>
+        <v>23730000</v>
       </c>
     </row>
   </sheetData>
@@ -14788,7 +14801,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -14798,7 +14811,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -14817,13 +14830,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -14834,10 +14847,10 @@
         <v>43113</v>
       </c>
       <c r="C5" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D5" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E5" s="4">
         <v>5000000</v>
@@ -14856,10 +14869,10 @@
         <v>43148</v>
       </c>
       <c r="C6" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D6" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E6" s="4">
         <v>5000000</v>

</xml_diff>